<commit_message>
Ran DRC and GGenerated Outputs
Zip files for PCB manufacturing were put together. Two DRC rules were added to the Main PCB file to eliminate related DRC Errors.
</commit_message>
<xml_diff>
--- a/Handheld DMX Console - V3/Default Configuration/Outputs/BOM/BOM_PartType-Handheld DMX Console - V3.xlsx
+++ b/Handheld DMX Console - V3/Default Configuration/Outputs/BOM/BOM_PartType-Handheld DMX Console - V3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{876BBC06-4D16-4129-B5CB-D1E25EAF1374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15D75A27-2076-4680-AE3F-9DF1F2AA216D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30405" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{54F1665F-4C9A-44FF-A7AC-B5D593BF10F5}"/>
+    <workbookView xWindow="30405" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{0DB8A0E8-E41A-4366-98B6-6AED07366911}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Handheld DMX Conso" sheetId="1" r:id="rId1"/>
@@ -704,7 +704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D218E0-C9EC-429D-A47E-0EF1216CD8FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAC47EC-BD09-4797-BFDF-6C4C17CBC9AF}">
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Added Silkscreen Order Number Marker
Added Indicators to hide order numbers from JLCPCB under parts
</commit_message>
<xml_diff>
--- a/Handheld DMX Console - V3/Default Configuration/Outputs/BOM/BOM_PartType-Handheld DMX Console - V3.xlsx
+++ b/Handheld DMX Console - V3/Default Configuration/Outputs/BOM/BOM_PartType-Handheld DMX Console - V3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15D75A27-2076-4680-AE3F-9DF1F2AA216D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D77A5B71-D23D-4213-B243-1876DE9A9C74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30405" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{0DB8A0E8-E41A-4366-98B6-6AED07366911}"/>
+    <workbookView xWindow="30405" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{A69E4006-9307-4AE5-AD67-715EF1D194D9}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Handheld DMX Conso" sheetId="1" r:id="rId1"/>
@@ -704,7 +704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAC47EC-BD09-4797-BFDF-6C4C17CBC9AF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117481F7-24E3-4347-8A07-C43A16A6158C}">
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>